<commit_message>
more data, first round regression models
</commit_message>
<xml_diff>
--- a/annual_midwest_soybean_yield.xlsx
+++ b/annual_midwest_soybean_yield.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laniepreston/Desktop/CapstoneCode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691F64CF-99AF-6740-8BC6-753873AF9ACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BE0E33-7299-7A46-9D1B-8066F955C09C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15960" xr2:uid="{94286BA1-FAE5-8942-B57E-F7DC7CF8A95F}"/>
+    <workbookView xWindow="17080" yWindow="980" windowWidth="27640" windowHeight="15960" xr2:uid="{94286BA1-FAE5-8942-B57E-F7DC7CF8A95F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,13 +390,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E96299-D397-854D-9102-09482819B6C3}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -408,321 +411,561 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1980</v>
+        <v>1950</v>
       </c>
       <c r="B2">
-        <v>25.8</v>
+        <v>20.2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1981</v>
+        <v>1951</v>
       </c>
       <c r="B3">
-        <v>28.3</v>
+        <v>19.8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1982</v>
+        <v>1952</v>
       </c>
       <c r="B4">
-        <v>27.5</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1983</v>
+        <v>1953</v>
       </c>
       <c r="B5">
-        <v>25.7</v>
+        <v>19.7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1984</v>
+        <v>1954</v>
       </c>
       <c r="B6">
-        <v>26.9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1985</v>
+        <v>1955</v>
       </c>
       <c r="B7">
-        <v>33.6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1986</v>
+        <v>1956</v>
       </c>
       <c r="B8">
-        <v>34.200000000000003</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1987</v>
+        <v>1957</v>
       </c>
       <c r="B9">
-        <v>30</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1988</v>
+        <v>1958</v>
       </c>
       <c r="B10">
-        <v>32.5</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1989</v>
+        <v>1959</v>
       </c>
       <c r="B11">
-        <v>32.5</v>
+        <v>22.6</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1990</v>
+        <v>1960</v>
       </c>
       <c r="B12">
-        <v>34</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1991</v>
+        <v>1961</v>
       </c>
       <c r="B13">
-        <v>34.700000000000003</v>
+        <v>25.1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1992</v>
+        <v>1962</v>
       </c>
       <c r="B14">
-        <v>37.5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1993</v>
+        <v>1963</v>
       </c>
       <c r="B15">
-        <v>32.5</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1994</v>
+        <v>1964</v>
       </c>
       <c r="B16">
-        <v>42.3</v>
+        <v>22.8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1995</v>
+        <v>1965</v>
       </c>
       <c r="B17">
-        <v>35.6</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>1996</v>
+        <v>1966</v>
       </c>
       <c r="B18">
-        <v>37.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1997</v>
+        <v>1967</v>
       </c>
       <c r="B19">
-        <v>49</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1998</v>
+        <v>1968</v>
       </c>
       <c r="B20">
-        <v>49</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1999</v>
+        <v>1969</v>
       </c>
       <c r="B21">
-        <v>36.200000000000003</v>
+        <v>26.3</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2000</v>
+        <v>1970</v>
       </c>
       <c r="B22">
-        <v>38</v>
+        <v>26.5</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>2001</v>
+        <v>1971</v>
       </c>
       <c r="B23">
-        <v>39.5</v>
+        <v>27.1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2002</v>
+        <v>1972</v>
       </c>
       <c r="B24">
-        <v>48</v>
+        <v>27.1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2003</v>
+        <v>1973</v>
       </c>
       <c r="B25">
-        <v>34</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2004</v>
+        <v>1974</v>
       </c>
       <c r="B26">
-        <v>43.7</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2005</v>
+        <v>1975</v>
       </c>
       <c r="B27">
-        <v>44.2</v>
+        <v>26.3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2006</v>
+        <v>1976</v>
       </c>
       <c r="B28">
-        <v>43</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2007</v>
+        <v>1977</v>
       </c>
       <c r="B29">
-        <v>42</v>
+        <v>28.4</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2008</v>
+        <v>1978</v>
       </c>
       <c r="B30">
-        <v>39.5</v>
+        <v>27.4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2009</v>
+        <v>1979</v>
       </c>
       <c r="B31">
-        <v>44.6</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>2010</v>
+        <v>1980</v>
       </c>
       <c r="B32">
-        <v>44</v>
+        <v>25.8</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2011</v>
+        <v>1981</v>
       </c>
       <c r="B33">
-        <v>42</v>
+        <v>28.3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2012</v>
+        <v>1982</v>
       </c>
       <c r="B34">
-        <v>40</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2013</v>
+        <v>1983</v>
       </c>
       <c r="B35">
-        <v>44.6</v>
+        <v>25.7</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>2014</v>
+        <v>1984</v>
       </c>
       <c r="B36">
-        <v>47.8</v>
+        <v>26.9</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>2015</v>
+        <v>1985</v>
       </c>
       <c r="B37">
-        <v>48</v>
+        <v>33.6</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>2016</v>
+        <v>1986</v>
       </c>
       <c r="B38">
-        <v>52.6</v>
+        <v>34.200000000000003</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>2017</v>
+        <v>1987</v>
       </c>
       <c r="B39">
-        <v>49.5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>2018</v>
+        <v>1988</v>
       </c>
       <c r="B40">
-        <v>52.3</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
+        <v>1989</v>
+      </c>
+      <c r="B41">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1990</v>
+      </c>
+      <c r="B42">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1991</v>
+      </c>
+      <c r="B43">
+        <v>34.700000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1992</v>
+      </c>
+      <c r="B44">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1993</v>
+      </c>
+      <c r="B45">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1994</v>
+      </c>
+      <c r="B46">
+        <v>42.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1995</v>
+      </c>
+      <c r="B47">
+        <v>35.6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1996</v>
+      </c>
+      <c r="B48">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1997</v>
+      </c>
+      <c r="B49">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1998</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1999</v>
+      </c>
+      <c r="B51">
+        <v>36.200000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2000</v>
+      </c>
+      <c r="B52">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2001</v>
+      </c>
+      <c r="B53">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2002</v>
+      </c>
+      <c r="B54">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2003</v>
+      </c>
+      <c r="B55">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2004</v>
+      </c>
+      <c r="B56">
+        <v>43.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2005</v>
+      </c>
+      <c r="B57">
+        <v>44.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2006</v>
+      </c>
+      <c r="B58">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2007</v>
+      </c>
+      <c r="B59">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2008</v>
+      </c>
+      <c r="B60">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2009</v>
+      </c>
+      <c r="B61">
+        <v>44.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2010</v>
+      </c>
+      <c r="B62">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2011</v>
+      </c>
+      <c r="B63">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2012</v>
+      </c>
+      <c r="B64">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2013</v>
+      </c>
+      <c r="B65">
+        <v>44.6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2014</v>
+      </c>
+      <c r="B66">
+        <v>47.8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2015</v>
+      </c>
+      <c r="B67">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2016</v>
+      </c>
+      <c r="B68">
+        <v>52.6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2017</v>
+      </c>
+      <c r="B69">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2018</v>
+      </c>
+      <c r="B70">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
         <v>2019</v>
       </c>
-      <c r="B41">
+      <c r="B71">
         <v>46.9</v>
       </c>
     </row>

</xml_diff>